<commit_message>
Minishop-001 | Create UI of Home Page to Customer able to access our application
</commit_message>
<xml_diff>
--- a/Planing Implement MiniShop.xlsx
+++ b/Planing Implement MiniShop.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Minishop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Minishop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5304" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5310"/>
   </bookViews>
   <sheets>
     <sheet name="Manage task" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Task</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Feb, 12: Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -571,18 +574,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -593,16 +596,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -613,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" t="s">
         <v>7</v>
@@ -622,7 +625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" t="s">
         <v>13</v>
@@ -631,73 +634,73 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
     </row>
   </sheetData>
@@ -718,19 +721,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -744,7 +747,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -754,139 +757,139 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -905,27 +908,27 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
@@ -944,14 +947,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>22</v>
       </c>
@@ -970,9 +973,9 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -993,7 +996,7 @@
       <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1012,7 +1015,7 @@
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1031,7 +1034,7 @@
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -1050,7 +1053,7 @@
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -1069,7 +1072,7 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -1088,7 +1091,7 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -1107,7 +1110,7 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1126,7 +1129,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -1145,7 +1148,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1164,7 +1167,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -1183,7 +1186,7 @@
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1202,7 +1205,7 @@
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1221,7 +1224,7 @@
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -1240,7 +1243,7 @@
       <c r="P14" s="9"/>
       <c r="Q14" s="9"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -1275,9 +1278,9 @@
       <selection sqref="A1:Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -1298,7 +1301,7 @@
       <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1317,7 +1320,7 @@
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1336,7 +1339,7 @@
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -1355,7 +1358,7 @@
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -1374,7 +1377,7 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -1393,7 +1396,7 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -1412,7 +1415,7 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1431,7 +1434,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -1450,7 +1453,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1469,7 +1472,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -1488,7 +1491,7 @@
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1507,7 +1510,7 @@
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1526,7 +1529,7 @@
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -1545,7 +1548,7 @@
       <c r="P14" s="9"/>
       <c r="Q14" s="9"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -1580,9 +1583,9 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
@@ -1603,7 +1606,7 @@
       <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1622,7 +1625,7 @@
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1641,7 +1644,7 @@
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -1660,7 +1663,7 @@
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -1679,7 +1682,7 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -1698,7 +1701,7 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -1717,7 +1720,7 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1736,7 +1739,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -1755,7 +1758,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1774,7 +1777,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -1793,7 +1796,7 @@
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1812,7 +1815,7 @@
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1831,7 +1834,7 @@
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -1850,7 +1853,7 @@
       <c r="P14" s="9"/>
       <c r="Q14" s="9"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>

</xml_diff>